<commit_message>
New net mesh calculation
</commit_message>
<xml_diff>
--- a/casting-net/Cast-Net-calculation.xlsx
+++ b/casting-net/Cast-Net-calculation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="330" windowWidth="19875" windowHeight="7710" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="330" windowWidth="19875" windowHeight="7710"/>
   </bookViews>
   <sheets>
     <sheet name="Расчет количества рядов" sheetId="1" r:id="rId1"/>
@@ -560,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -963,8 +963,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>